<commit_message>
Adjust Investment Problem and add standard output
Add tec and gtec sets
Fix vGenInvest to be Integer values
</commit_message>
<xml_diff>
--- a/data/NREL-118 7 clusters Investment/Power_Storage.xlsx
+++ b/data/NREL-118 7 clusters Investment/Power_Storage.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\NREL-118 7 clusters Investment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF82C68A-73B6-408A-AEAC-6A18AC5C6E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFCB3EA-88EC-418B-BA0D-16E804F3D6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11790" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -437,26 +450,31 @@
       <b/>
       <sz val="11"/>
       <name val="Aptos"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <name val="Aptos"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Aptos"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color rgb="FFFFFFFF"/>
       <name val="Aptos"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -869,10 +887,10 @@
   <dimension ref="A1:AD9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="T8" s="13">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="U8" s="15">
         <v>3821.0756000000001</v>
@@ -1500,7 +1518,7 @@
         <v>1</v>
       </c>
       <c r="T9" s="13">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="U9" s="15">
         <v>3821.0756000000001</v>

</xml_diff>